<commit_message>
excel photo notes column added
</commit_message>
<xml_diff>
--- a/testData/productData.xlsx
+++ b/testData/productData.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC89016F-356C-4392-A358-86E8EBF6B8B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="15375" windowHeight="7785"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="2" name="USA Markdowns" state="visible" r:id="rId4"/>
+    <sheet name="USA Markdowns" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>USA Markdowns</t>
   </si>
@@ -99,58 +100,63 @@
   <si>
     <t xml:space="preserve">Product validation skipped as Colour not found -&gt; Expected Color "Black" for "Steady State Pullover Hoodie *Collegiate" was not present. </t>
   </si>
+  <si>
+    <t>Photo Notes</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b/>
+      <sz val="23"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
-      <sz val="16"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <color rgb="FF000000"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <color rgb="FFFFFFFF"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-      <sz val="12"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <color rgb="FF000000"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-    </font>
-    <font>
-      <color rgb="FF000000"/>
-      <family val="2"/>
-      <sz val="23"/>
-      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="4">
@@ -512,21 +518,21 @@
 </a:theme>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P381"/>
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q381"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25" defaultColWidth="20.42578125"/>
+  <sheetFormatPr defaultColWidth="20.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="28.7109375" customWidth="1"/>
     <col min="13" max="13" width="20.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="21" customHeight="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -545,8 +551,9 @@
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
       <c r="P1" s="3"/>
-    </row>
-    <row r="2" ht="15.75" customHeight="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q1" s="3"/>
+    </row>
+    <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -595,8 +602,11 @@
       <c r="P2" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" ht="30" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q2" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>17</v>
       </c>
@@ -637,7 +647,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
@@ -652,7 +662,7 @@
       <c r="L4" s="7"/>
       <c r="M4" s="8"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -667,7 +677,7 @@
       <c r="L5" s="7"/>
       <c r="M5" s="8"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -682,7 +692,7 @@
       <c r="L6" s="7"/>
       <c r="M6" s="8"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -697,7 +707,7 @@
       <c r="L7" s="7"/>
       <c r="M7" s="8"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -712,7 +722,7 @@
       <c r="L8" s="7"/>
       <c r="M8" s="8"/>
     </row>
-    <row r="9" ht="29.25" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -727,7 +737,7 @@
       <c r="L9" s="7"/>
       <c r="M9" s="8"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -742,7 +752,7 @@
       <c r="L10" s="7"/>
       <c r="M10" s="8"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -757,7 +767,7 @@
       <c r="L11" s="7"/>
       <c r="M11" s="8"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -772,7 +782,7 @@
       <c r="L12" s="7"/>
       <c r="M12" s="8"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -787,7 +797,7 @@
       <c r="L13" s="7"/>
       <c r="M13" s="8"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
@@ -802,7 +812,7 @@
       <c r="L14" s="7"/>
       <c r="M14" s="8"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -817,7 +827,7 @@
       <c r="L15" s="7"/>
       <c r="M15" s="8"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -5776,7 +5786,7 @@
       <c r="K368" s="5"/>
       <c r="L368" s="7"/>
     </row>
-    <row r="369" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A369" s="7"/>
       <c r="B369" s="7"/>
       <c r="C369" s="7"/>
@@ -5790,7 +5800,7 @@
       <c r="K369" s="5"/>
       <c r="L369" s="7"/>
     </row>
-    <row r="370" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A370" s="7"/>
       <c r="B370" s="7"/>
       <c r="C370" s="7"/>
@@ -5804,7 +5814,7 @@
       <c r="K370" s="5"/>
       <c r="L370" s="7"/>
     </row>
-    <row r="371" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A371" s="7"/>
       <c r="B371" s="7"/>
       <c r="C371" s="7"/>
@@ -5818,7 +5828,7 @@
       <c r="K371" s="5"/>
       <c r="L371" s="7"/>
     </row>
-    <row r="372" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A372" s="7"/>
       <c r="B372" s="7"/>
       <c r="C372" s="7"/>
@@ -5832,7 +5842,7 @@
       <c r="K372" s="5"/>
       <c r="L372" s="7"/>
     </row>
-    <row r="373" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A373" s="7"/>
       <c r="B373" s="7"/>
       <c r="C373" s="7"/>
@@ -5846,7 +5856,7 @@
       <c r="K373" s="5"/>
       <c r="L373" s="7"/>
     </row>
-    <row r="374" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A374" s="7"/>
       <c r="B374" s="7"/>
       <c r="C374" s="7"/>
@@ -5860,7 +5870,7 @@
       <c r="K374" s="5"/>
       <c r="L374" s="7"/>
     </row>
-    <row r="375" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A375" s="7"/>
       <c r="B375" s="7"/>
       <c r="C375" s="7"/>
@@ -5874,7 +5884,7 @@
       <c r="K375" s="5"/>
       <c r="L375" s="7"/>
     </row>
-    <row r="376" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A376" s="7"/>
       <c r="B376" s="7"/>
       <c r="C376" s="7"/>
@@ -5888,7 +5898,7 @@
       <c r="K376" s="5"/>
       <c r="L376" s="7"/>
     </row>
-    <row r="377" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A377" s="7"/>
       <c r="B377" s="7"/>
       <c r="C377" s="7"/>
@@ -5902,7 +5912,7 @@
       <c r="K377" s="5"/>
       <c r="L377" s="7"/>
     </row>
-    <row r="378" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A378" s="7"/>
       <c r="B378" s="7"/>
       <c r="C378" s="7"/>
@@ -5916,7 +5926,7 @@
       <c r="K378" s="5"/>
       <c r="L378" s="7"/>
     </row>
-    <row r="379" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A379" s="7"/>
       <c r="B379" s="7"/>
       <c r="C379" s="7"/>
@@ -5930,7 +5940,7 @@
       <c r="K379" s="5"/>
       <c r="L379" s="7"/>
     </row>
-    <row r="380" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A380" s="7"/>
       <c r="B380" s="7"/>
       <c r="C380" s="7"/>
@@ -5944,11 +5954,11 @@
       <c r="K380" s="5"/>
       <c r="L380" s="7"/>
     </row>
-    <row r="381" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M381" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
</xml_diff>